<commit_message>
Revert "Merge branch 'main' into Big-Map-Pathfinding"
This reverts commit 3c0e3e4318f97381544dd97defa7f1145a82624c, reversing
changes made to d596c2b2ec35ea93a35485b2aa551bbda0cc134b.
</commit_message>
<xml_diff>
--- a/Keep Eating Acceptance QA Testing doc.xlsx
+++ b/Keep Eating Acceptance QA Testing doc.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/50680cce39607b31/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CB139539-516D-43A4-BBB6-AB8F512EE70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="14_{B712EE41-6E9A-4F3F-AE9E-A92FEF3BCC3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
   <si>
     <t>Project Name</t>
   </si>
@@ -73,6 +73,9 @@
   </si>
   <si>
     <t>Keep Eating</t>
+  </si>
+  <si>
+    <t>Darnell Faison</t>
   </si>
   <si>
     <r>
@@ -121,26 +124,6 @@
     <t>That name will appear with the user's character sprite in the lobby and in the game.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t xml:space="preserve">Create Lobby
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color indexed="8"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>Create a unique lobby code for other's to join your game.</t>
-    </r>
-  </si>
-  <si>
     <t>User will enter a lobby that can only be accessed via the unique code the user created. Anyone who joins the lobby will appear here until the game starts.</t>
   </si>
   <si>
@@ -162,22 +145,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Join lobby w/o unique lobby code </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Helvetica Neue"/>
-      </rPr>
-      <t>User joins a lobby with a random lobby code.</t>
-    </r>
-  </si>
-  <si>
-    <t>User will enter a lobby with a random lobby code and anyone else who joins without a lobby code will be placed in this same lobby.</t>
-  </si>
-  <si>
-    <r>
       <t xml:space="preserve">Join Enforcer
 </t>
     </r>
@@ -299,7 +266,173 @@
     <t>After an Eater dies, the player will respawn on the map with a full health bar.</t>
   </si>
   <si>
-    <t>Darnell Faison (darnell.faison@temple.edu)</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve">Create Lobby by entering code
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color indexed="8"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Create a unique lobby code for other's to join your game.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Create lobby w/o unique lobby code </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>User creates a lobby without entering a code</t>
+    </r>
+  </si>
+  <si>
+    <t>User will enter a lobby with a random lobby code and anyone else who joins without a lobby code will be placed in this same lobby. The random new lobby code can also be used by other's to join the same lobby.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Eaters pick up taser
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Eater player can pick the taser weapon</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>by pressing the "F" key</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Eaters shoot taser
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>Eaters can shoot the taser once they have it picked up via mouse click</t>
+    </r>
+  </si>
+  <si>
+    <t>Eaters can freeze Enforcers by hitting them with the taser.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Change game settings
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>When  in the lobby, the game master can change the game settings by clicking on the settings option.</t>
+    </r>
+  </si>
+  <si>
+    <t>A menu will appear allowing the game master to change the game's settings.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Change map
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>If game master changes the map fromt the settings menu, the game will be played on the slected map.</t>
+    </r>
+  </si>
+  <si>
+    <t>Game will load on the small map if "small map" is selected or on the big map if "big map" is selected.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Allow bots
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>User can allow for bots to play in the game as interactive players.</t>
+    </r>
+  </si>
+  <si>
+    <t>When the game loads, bots will be playing their roles as either "Eater" or "Enforcer"</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Set to private
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>If the game master sets the game to private via the settings menu, no one can publicly join the lobby</t>
+    </r>
+  </si>
+  <si>
+    <t>Other user's cannot use the lobby code to enter the game master's lobby</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Match ends
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Helvetica Neue"/>
+      </rPr>
+      <t>When either the "Eaters" reach their goal or time runs out, a winner is determind and the match ends</t>
+    </r>
+  </si>
+  <si>
+    <t>When the match ends, a winner is determind and the players return to the game lobby.</t>
   </si>
 </sst>
 </file>
@@ -1707,8 +1840,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.28515625" defaultRowHeight="19.899999999999999" customHeight="1"/>
@@ -1739,7 +1872,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>39</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
@@ -1802,7 +1935,7 @@
         <v>12</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>9</v>
@@ -1813,10 +1946,10 @@
         <v>1</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
@@ -1826,10 +1959,10 @@
         <v>2</v>
       </c>
       <c r="B8" s="16" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D8" s="18"/>
       <c r="E8" s="18"/>
@@ -1839,7 +1972,7 @@
         <v>3</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>19</v>
@@ -1865,10 +1998,10 @@
         <v>5</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>23</v>
+        <v>39</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15"/>
@@ -1878,10 +2011,10 @@
         <v>6</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>24</v>
+        <v>43</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>25</v>
+        <v>44</v>
       </c>
       <c r="D12" s="15"/>
       <c r="E12" s="15"/>
@@ -1891,110 +2024,170 @@
         <v>7</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>26</v>
+        <v>45</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>27</v>
+        <v>46</v>
       </c>
       <c r="D13" s="15"/>
       <c r="E13" s="15"/>
     </row>
     <row r="14" spans="1:5" ht="126.6" customHeight="1">
       <c r="A14" s="12">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15"/>
     </row>
     <row r="15" spans="1:5" ht="126.6" customHeight="1">
       <c r="A15" s="12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>28</v>
+        <v>49</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
     </row>
     <row r="16" spans="1:5" ht="126.6" customHeight="1">
       <c r="A16" s="12">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="D16" s="15"/>
       <c r="E16" s="15"/>
     </row>
     <row r="17" spans="1:5" ht="126.6" customHeight="1">
       <c r="A17" s="12">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="D17" s="15"/>
       <c r="E17" s="15"/>
     </row>
     <row r="18" spans="1:5" ht="126.6" customHeight="1">
       <c r="A18" s="12">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="D18" s="15"/>
       <c r="E18" s="15"/>
     </row>
     <row r="19" spans="1:5" ht="126.6" customHeight="1">
       <c r="A19" s="12">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C19" s="14" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="D19" s="15"/>
       <c r="E19" s="15"/>
     </row>
     <row r="20" spans="1:5" ht="126.6" customHeight="1">
       <c r="A20" s="12">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C20" s="14" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D20" s="15"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:5" ht="126.6" customHeight="1"/>
-    <row r="22" spans="1:5" ht="126.6" customHeight="1"/>
-    <row r="23" spans="1:5" ht="126.6" customHeight="1"/>
-    <row r="24" spans="1:5" ht="126.6" customHeight="1"/>
-    <row r="25" spans="1:5" ht="126.6" customHeight="1"/>
+    <row r="21" spans="1:5" ht="126.6" customHeight="1">
+      <c r="A21" s="12">
+        <v>15</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+    </row>
+    <row r="22" spans="1:5" ht="126.6" customHeight="1">
+      <c r="A22" s="12">
+        <v>16</v>
+      </c>
+      <c r="B22" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22" s="15"/>
+      <c r="E22" s="15"/>
+    </row>
+    <row r="23" spans="1:5" ht="126.6" customHeight="1">
+      <c r="A23" s="12">
+        <v>17</v>
+      </c>
+      <c r="B23" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="D23" s="15"/>
+      <c r="E23" s="15"/>
+    </row>
+    <row r="24" spans="1:5" ht="126.6" customHeight="1">
+      <c r="A24" s="12">
+        <v>18</v>
+      </c>
+      <c r="B24" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24" s="15"/>
+      <c r="E24" s="15"/>
+    </row>
+    <row r="25" spans="1:5" ht="126.6" customHeight="1">
+      <c r="A25" s="12">
+        <v>19</v>
+      </c>
+      <c r="B25" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="15"/>
+      <c r="E25" s="15"/>
+    </row>
     <row r="26" spans="1:5" ht="126.6" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.27777800000000002" footer="0.27777800000000002"/>

</xml_diff>